<commit_message>
modificacion y remasterización ademas de trabajo con git
</commit_message>
<xml_diff>
--- a/src/test/java/viajesfalabella/equipo1/Equipo 1.xlsx
+++ b/src/test/java/viajesfalabella/equipo1/Equipo 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tsoftlatam-my.sharepoint.com/personal/christian_lopez_tsoftglobal_com/Documents/Archivos de chat de Microsoft Teams/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian.Lopez\IdeaProjects\bootcamp-2021-5-CLopez\src\test\java\viajesfalabella\equipo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="13_ncr:1_{EBC14840-9C1E-4345-B2F4-E931EC5E3F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F955E2F-85FF-42EE-ABEC-3FEFFD605EB2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFA693F-5D31-4746-95C6-9F2C0DDB3F3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8148" xr2:uid="{0627F527-14F2-4417-8134-FCDB25AE22D1}"/>
+    <workbookView xWindow="1170" yWindow="0" windowWidth="19200" windowHeight="8145" xr2:uid="{0627F527-14F2-4417-8134-FCDB25AE22D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -632,7 +623,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -657,7 +648,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -667,6 +658,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -712,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -753,6 +756,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -792,7 +815,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1090,11 +1113,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419BA8B9-A41D-4ECE-811F-18902A89CB9B}">
   <dimension ref="B4:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
@@ -1105,7 +1128,7 @@
     <col min="7" max="8" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="351" customHeight="1">
+    <row r="5" spans="2:8" ht="351" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1148,7 +1171,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="271.5" customHeight="1">
+    <row r="6" spans="2:8" ht="271.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1169,7 +1192,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="2:8" ht="303.95" customHeight="1">
+    <row r="7" spans="2:8" ht="303.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1189,7 +1212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="351.95" customHeight="1">
+    <row r="8" spans="2:8" ht="351.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1209,7 +1232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="314.10000000000002" customHeight="1">
+    <row r="9" spans="2:8" ht="314.10000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1229,7 +1252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="180.6" customHeight="1">
+    <row r="10" spans="2:8" ht="180.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1249,27 +1272,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="341.1" customHeight="1">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:8" s="17" customFormat="1" ht="341.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="195">
+    <row r="12" spans="2:8" ht="180" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1289,27 +1312,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="150">
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="2:8" s="21" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="254.45" customHeight="1">
+    <row r="14" spans="2:8" ht="254.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
@@ -1329,7 +1352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="330" customHeight="1">
+    <row r="15" spans="2:8" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
@@ -1349,7 +1372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="190.5" customHeight="1">
+    <row r="16" spans="2:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>47</v>
       </c>

</xml_diff>